<commit_message>
fix for problem data extraction
</commit_message>
<xml_diff>
--- a/openrouter_resume_data.xlsx
+++ b/openrouter_resume_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,370 +436,227 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>File Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Extraction Method</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name of Candidate</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Birth Date</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Marital Status</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Permanent Address</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Contact Number</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Email ID</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Education</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Total Years of Experience</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Experience Details</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Current Monthly Salary</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>District</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Present Address</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>PAN Card</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Aadhar Card</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>State</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Preferred Job Location</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>File Name</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PADSALA DENISH VINUBHAI</t>
+          <t>DENISH RESUME.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>13/04/2000</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Unmarried</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>AT- VANDALIYA PIN - 365421 TA - BABRA Dist - AMRELI</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>91 9687765151</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>denipadsala7@gmail.com</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>S.S.C. from GSHEB, March 2016; H.S.C. from GSHEB, March 2019; B.Com from Saurashtra University, 2022</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>VIDEOCON D2H (6 Month Field Sales)</t>
-        </is>
-      </c>
+          <t>Native</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>AMRELI</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>DENISH RESUME.pdf</t>
-        </is>
-      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Praful N Matang</t>
+          <t>praful n matang.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14-03-1998</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Marride</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Vill- Nani Khakhar Mandvi Kutch Gujarat 370435</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>91 6359051032</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>prafulmatan mail.com</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Nani Khakhar 2011 Pass; I.TIWELDER Mandvi ITi 2017 Pass</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Surveyor at Masmarine Services India Pvt Ltd for 5 years; Technician at Adani Solar Ingot Wefer Plant (Mundra) for 1 year</t>
-        </is>
-      </c>
+          <t>Native</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Kutch</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>praful n matang.pdf</t>
-        </is>
-      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Saharvadi Noormamad</t>
+          <t>97239 95928 CV.pdf</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11/09/1982</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Married</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Near Hanuman Temple, Gandhinagari, Okha Port 361350</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>491 97239 95928</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>jaanoomd68@gmail.com</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>S.S.C. (Gujarat Secondary Education Board, 2013), ITI (Director of Employment Training Gujarat Council of Vocational Training, 2002-2004), Wireman Certificate (30 Jan 2006), National Trade Certificate (July 2004), Lineman Certificate (PGVCL Okha Sub., 05 Apr 2010 - 04 Apr 2012), National Apprenticeship Certificate (National Council for Vocational Training, 05 Apr 2010 - 04 Apr 2012)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>13 years</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Worked as DG Set Operator with Indian Navy (INS Dwarka) from Aug 2004 to Jan 2009, Field Supervisor with Asian Marine (Okha) from Apr 2014 to Dec 2017, and LT 11kv Line Field Maintenance Supervisor with PGVCL Under Contract Shree Bhagvati Construction (Bhimrana) from Jan 2018 to Dec 2022, handling electrical equipment maintenance, repair, and field supervision across naval and civilian projects.</t>
-        </is>
-      </c>
+          <t>Native</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Okha</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>97239 95928 CV.pdf</t>
-        </is>
-      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AKASH KUMAR SAMANTA</t>
+          <t>Akash Samanta.pdf</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17/04/2004</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Unmarried</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Vill-Chandanpur, P.O- Radhachandanpur, P:S- Debra PIN-721160, DIST- PASCHIM MEDINIPUR STATE- WEST:BENGAL</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>918348493162</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>akashsamanta30666@gmail.com</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Secondary (B.B) 2020, Higher Secondary (S.E) 2022, Diploma (DITA) 2025</t>
-        </is>
-      </c>
+          <t>Native</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>PASCHIM MEDINIPUR</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>West Bengal</t>
-        </is>
-      </c>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Akash Samanta.pdf</t>
-        </is>
-      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>9904335536.pdf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Native</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
@@ -815,15 +672,20 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>9904335536.pdf</t>
-        </is>
-      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sagar.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Native</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
@@ -839,155 +701,66 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>sagar.pdf</t>
-        </is>
-      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bharat Singh</t>
+          <t>Bharat  singh cv pdf (1).pdf</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21/06/2006</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>UN-MARRIED</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>VPO-MAHESHO KI DHANI TEH.-POKARAN ,JAISALMER RAJASTHAN 345023</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>9636084189</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>bharatsabhati52@gmail.com</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>10th grade from RBSE Ajmer (2022); Two-year ITI Electrician from NCVT Govt. ITI Pokaran Jaisalmer (2023-24)</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>1.4</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Site Technician with 1.4 months experience in Solar Project; Project Leader at SSB Enterprises, Rampur Chok; Technician - Electrical; responsibilities include AC/DC cable, inverter, transformer cable laying, PV module string to string combiner box, etc.</t>
-        </is>
-      </c>
+          <t>Native</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>JAISALMER</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>MALE</t>
-        </is>
-      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>RAJASTHAN</t>
-        </is>
-      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Bharat  singh cv pdf (1).pdf</t>
-        </is>
-      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SHARMA RAVI R.</t>
+          <t>6354451986.pdf</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17-12-2000</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Unmarried</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Krishna Sheri, Vachlu Faliyu, Danteshwar, Pratapanagar, Vadodara- 390004</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>6354451986</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>sharmaraviil234@gmail.com</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>SSC GSEB 2017 53.66%, HSC GSHEB 2019 50.71%, ITI(TURNER) NCVT 2021 70.50%</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>1 Year Vmc Machine Operator (Microfine Products)</t>
-        </is>
-      </c>
+          <t>Native</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Vadodara</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>6354451986.pdf</t>
-        </is>
-      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>